<commit_message>
Element 2 collapse and Dual override
</commit_message>
<xml_diff>
--- a/Master Migration Rules.xlsx
+++ b/Master Migration Rules.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CLANCE\Documents\Syncplicity Folders\Livingston\_CODA Initiative - Hermes\Migration\Baseline\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CLANCE\Documents\Syncplicity Folders\Livingston\_CODA Initiative - Hermes\Migration\PDI\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -79,7 +79,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I25" authorId="0" shapeId="0">
+    <comment ref="I28" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -103,7 +103,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J35" authorId="0" shapeId="0">
+    <comment ref="J38" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -132,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="273">
   <si>
     <t>Section</t>
   </si>
@@ -948,6 +948,9 @@
   </si>
   <si>
     <t>CMPCODE,YR</t>
+  </si>
+  <si>
+    <t>Renamed DB Copy</t>
   </si>
 </sst>
 </file>
@@ -1103,30 +1106,9 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="3">
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -1153,9 +1135,6 @@
         <scheme val="minor"/>
       </font>
     </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1170,10 +1149,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:O55" totalsRowShown="0" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:O55" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A1:O55"/>
-  <sortState ref="A11:P48">
-    <sortCondition sortBy="cellColor" ref="F1:F55" dxfId="3"/>
+  <sortState ref="A2:O55">
+    <sortCondition ref="D1:D55"/>
   </sortState>
   <tableColumns count="15">
     <tableColumn id="1" name="In Requel List"/>
@@ -1182,7 +1161,7 @@
     <tableColumn id="4" name="Section"/>
     <tableColumn id="5" name="Type"/>
     <tableColumn id="6" name="Migration Method"/>
-    <tableColumn id="7" name="Truncate Dest" dataDxfId="5"/>
+    <tableColumn id="7" name="Truncate Dest" dataDxfId="0"/>
     <tableColumn id="8" name="XMLi Service"/>
     <tableColumn id="9" name="Header Table"/>
     <tableColumn id="10" name="Detail Table 1"/>
@@ -1461,8 +1440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D22" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1910,7 +1889,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B11" t="s">
         <v>80</v>
@@ -1919,36 +1898,36 @@
         <v>80</v>
       </c>
       <c r="D11" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="E11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>246</v>
+        <v>44</v>
+      </c>
+      <c r="F11" t="s">
+        <v>258</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H11" t="s">
-        <v>105</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>163</v>
+        <v>125</v>
+      </c>
+      <c r="I11" t="s">
+        <v>85</v>
+      </c>
+      <c r="J11" t="s">
+        <v>206</v>
       </c>
       <c r="L11" t="s">
         <v>164</v>
       </c>
       <c r="M11" t="s">
-        <v>165</v>
+        <v>210</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B12" t="s">
         <v>80</v>
@@ -1957,540 +1936,453 @@
         <v>80</v>
       </c>
       <c r="D12" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="E12" t="s">
-        <v>4</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>254</v>
+        <v>45</v>
+      </c>
+      <c r="F12" t="s">
+        <v>258</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H12" t="s">
-        <v>99</v>
+        <v>126</v>
       </c>
       <c r="I12" t="s">
-        <v>166</v>
+        <v>86</v>
       </c>
       <c r="J12" t="s">
-        <v>152</v>
-      </c>
-      <c r="K12" t="s">
-        <v>152</v>
+        <v>207</v>
       </c>
       <c r="L12" t="s">
         <v>164</v>
       </c>
+      <c r="M12" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>80</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>103</v>
+      <c r="B13" t="s">
+        <v>80</v>
       </c>
       <c r="C13" t="s">
         <v>80</v>
       </c>
       <c r="D13" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="E13" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>246</v>
+        <v>46</v>
+      </c>
+      <c r="F13" t="s">
+        <v>258</v>
       </c>
       <c r="G13" s="12" t="s">
         <v>80</v>
       </c>
       <c r="H13" t="s">
-        <v>109</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="K13" s="5" t="s">
-        <v>174</v>
+        <v>127</v>
+      </c>
+      <c r="I13" t="s">
+        <v>87</v>
       </c>
       <c r="L13" t="s">
-        <v>135</v>
-      </c>
-      <c r="M13" t="s">
-        <v>175</v>
-      </c>
-      <c r="N13" t="s">
-        <v>175</v>
-      </c>
-      <c r="O13" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>80</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C14" t="s">
-        <v>79</v>
-      </c>
       <c r="D14" t="s">
-        <v>5</v>
+        <v>227</v>
       </c>
       <c r="E14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>246</v>
+        <v>223</v>
+      </c>
+      <c r="F14" t="s">
+        <v>267</v>
       </c>
       <c r="G14" s="12" t="s">
         <v>80</v>
       </c>
       <c r="H14" t="s">
-        <v>110</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="J14" s="5" t="s">
-        <v>177</v>
+        <v>229</v>
+      </c>
+      <c r="I14" t="s">
+        <v>234</v>
+      </c>
+      <c r="J14" t="s">
+        <v>236</v>
+      </c>
+      <c r="K14" t="s">
+        <v>240</v>
       </c>
       <c r="L14" t="s">
         <v>164</v>
       </c>
       <c r="M14" t="s">
-        <v>178</v>
+        <v>238</v>
+      </c>
+      <c r="N14" t="s">
+        <v>238</v>
+      </c>
+      <c r="O14" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>80</v>
-      </c>
-      <c r="B15" t="s">
-        <v>79</v>
-      </c>
-      <c r="C15" t="s">
-        <v>79</v>
-      </c>
       <c r="D15" t="s">
-        <v>20</v>
+        <v>227</v>
       </c>
       <c r="E15" t="s">
-        <v>21</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>246</v>
+        <v>224</v>
+      </c>
+      <c r="F15" t="s">
+        <v>267</v>
       </c>
       <c r="G15" s="12" t="s">
         <v>80</v>
       </c>
       <c r="H15" t="s">
-        <v>117</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="J15" s="5" t="s">
-        <v>252</v>
+        <v>232</v>
+      </c>
+      <c r="I15" t="s">
+        <v>239</v>
       </c>
       <c r="L15" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>80</v>
-      </c>
-      <c r="B16" t="s">
-        <v>79</v>
-      </c>
-      <c r="C16" t="s">
-        <v>79</v>
-      </c>
       <c r="D16" t="s">
-        <v>30</v>
+        <v>227</v>
       </c>
       <c r="E16" t="s">
-        <v>36</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>246</v>
+        <v>225</v>
+      </c>
+      <c r="F16" t="s">
+        <v>267</v>
       </c>
       <c r="G16" s="12" t="s">
         <v>80</v>
       </c>
       <c r="H16" t="s">
-        <v>222</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="J16" s="5" t="s">
-        <v>215</v>
+        <v>233</v>
+      </c>
+      <c r="I16" t="s">
+        <v>237</v>
       </c>
       <c r="L16" t="s">
         <v>164</v>
       </c>
-      <c r="M16" t="s">
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D17" t="s">
+        <v>227</v>
+      </c>
+      <c r="E17" t="s">
+        <v>226</v>
+      </c>
+      <c r="F17" t="s">
+        <v>267</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="H17" t="s">
+        <v>230</v>
+      </c>
+      <c r="I17" t="s">
+        <v>235</v>
+      </c>
+      <c r="L17" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>80</v>
-      </c>
-      <c r="B17" t="s">
-        <v>80</v>
-      </c>
-      <c r="C17" t="s">
-        <v>79</v>
-      </c>
-      <c r="D17" t="s">
-        <v>30</v>
-      </c>
-      <c r="E17" t="s">
-        <v>38</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="G17" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="H17" t="s">
-        <v>218</v>
-      </c>
-      <c r="I17" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="J17" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="L17" t="s">
-        <v>199</v>
-      </c>
-      <c r="M17" t="s">
-        <v>200</v>
-      </c>
-    </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>80</v>
-      </c>
-      <c r="B18" t="s">
-        <v>79</v>
-      </c>
-      <c r="C18" t="s">
-        <v>80</v>
-      </c>
       <c r="D18" t="s">
-        <v>30</v>
+        <v>227</v>
       </c>
       <c r="E18" t="s">
-        <v>39</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>246</v>
+        <v>243</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>267</v>
       </c>
       <c r="G18" s="12" t="s">
         <v>80</v>
       </c>
       <c r="H18" t="s">
-        <v>219</v>
-      </c>
-      <c r="I18" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="J18" s="7" t="s">
-        <v>68</v>
+        <v>104</v>
+      </c>
+      <c r="I18" t="s">
+        <v>269</v>
+      </c>
+      <c r="J18" t="s">
+        <v>270</v>
       </c>
       <c r="L18" t="s">
-        <v>164</v>
+        <v>271</v>
       </c>
       <c r="M18" t="s">
-        <v>164</v>
+        <v>271</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>80</v>
-      </c>
-      <c r="B19" t="s">
-        <v>80</v>
-      </c>
-      <c r="C19" t="s">
-        <v>80</v>
-      </c>
       <c r="D19" t="s">
-        <v>30</v>
+        <v>227</v>
       </c>
       <c r="E19" t="s">
-        <v>40</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>246</v>
+        <v>228</v>
+      </c>
+      <c r="F19" t="s">
+        <v>267</v>
       </c>
       <c r="G19" s="12" t="s">
         <v>80</v>
       </c>
       <c r="H19" t="s">
-        <v>220</v>
-      </c>
-      <c r="I19" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="J19" s="7" t="s">
-        <v>70</v>
+        <v>231</v>
+      </c>
+      <c r="I19" t="s">
+        <v>241</v>
       </c>
       <c r="L19" t="s">
         <v>164</v>
       </c>
-      <c r="M19" t="s">
-        <v>202</v>
-      </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B20" t="s">
         <v>80</v>
       </c>
       <c r="C20" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D20" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E20" t="s">
-        <v>6</v>
-      </c>
-      <c r="F20" t="s">
-        <v>258</v>
+        <v>3</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>246</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H20" t="s">
-        <v>106</v>
-      </c>
-      <c r="I20" t="s">
-        <v>167</v>
-      </c>
-      <c r="J20" t="s">
-        <v>168</v>
+        <v>105</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>163</v>
       </c>
       <c r="L20" t="s">
-        <v>135</v>
+        <v>164</v>
       </c>
       <c r="M20" t="s">
-        <v>135</v>
+        <v>165</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B21" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C21" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D21" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E21" t="s">
-        <v>7</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>246</v>
+        <v>4</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>272</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H21" t="s">
-        <v>107</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>170</v>
+        <v>99</v>
+      </c>
+      <c r="I21" t="s">
+        <v>166</v>
+      </c>
+      <c r="J21" t="s">
+        <v>152</v>
+      </c>
+      <c r="K21" t="s">
+        <v>152</v>
       </c>
       <c r="L21" t="s">
-        <v>135</v>
-      </c>
-      <c r="M21" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B22" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="C22" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
       <c r="D22" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="E22" t="s">
-        <v>10</v>
-      </c>
-      <c r="F22" t="s">
-        <v>258</v>
+        <v>48</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>247</v>
       </c>
       <c r="G22" s="12" t="s">
         <v>80</v>
       </c>
       <c r="H22" t="s">
-        <v>111</v>
+        <v>128</v>
       </c>
       <c r="I22" t="s">
-        <v>180</v>
-      </c>
-      <c r="J22" t="s">
-        <v>183</v>
+        <v>214</v>
       </c>
       <c r="L22" t="s">
-        <v>135</v>
-      </c>
-      <c r="M22" t="s">
-        <v>135</v>
+        <v>164</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>79</v>
-      </c>
-      <c r="B23" t="s">
-        <v>104</v>
+        <v>80</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>103</v>
       </c>
       <c r="C23" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="D23" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="E23" t="s">
-        <v>18</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>247</v>
+        <v>8</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>242</v>
       </c>
       <c r="G23" s="12" t="s">
         <v>80</v>
       </c>
       <c r="H23" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="I23" t="s">
-        <v>211</v>
+        <v>172</v>
       </c>
       <c r="J23" t="s">
-        <v>212</v>
+        <v>173</v>
+      </c>
+      <c r="K23" t="s">
+        <v>174</v>
       </c>
       <c r="L23" t="s">
-        <v>164</v>
+        <v>135</v>
       </c>
       <c r="M23" t="s">
-        <v>213</v>
+        <v>175</v>
+      </c>
+      <c r="N23" t="s">
+        <v>175</v>
+      </c>
+      <c r="O23" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>79</v>
-      </c>
-      <c r="B24" t="s">
-        <v>104</v>
+        <v>80</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>103</v>
       </c>
       <c r="C24" t="s">
-        <v>104</v>
+        <v>79</v>
       </c>
       <c r="D24" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="E24" t="s">
-        <v>19</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>247</v>
+        <v>9</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>242</v>
       </c>
       <c r="G24" s="12" t="s">
         <v>80</v>
       </c>
       <c r="H24" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="I24" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="J24" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="L24" t="s">
         <v>164</v>
       </c>
       <c r="M24" t="s">
-        <v>201</v>
+        <v>178</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>80</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>103</v>
+      <c r="B25" t="s">
+        <v>80</v>
       </c>
       <c r="C25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D25" t="s">
         <v>5</v>
       </c>
       <c r="E25" t="s">
-        <v>11</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>246</v>
+        <v>6</v>
+      </c>
+      <c r="F25" t="s">
+        <v>258</v>
       </c>
       <c r="G25" s="12" t="s">
         <v>80</v>
       </c>
       <c r="H25" t="s">
-        <v>112</v>
-      </c>
-      <c r="I25" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>61</v>
+        <v>106</v>
+      </c>
+      <c r="I25" t="s">
+        <v>167</v>
+      </c>
+      <c r="J25" t="s">
+        <v>168</v>
       </c>
       <c r="L25" t="s">
-        <v>164</v>
+        <v>135</v>
       </c>
       <c r="M25" t="s">
-        <v>184</v>
-      </c>
-      <c r="N25" t="s">
-        <v>184</v>
-      </c>
-      <c r="O25" t="s">
-        <v>160</v>
+        <v>135</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
@@ -2498,16 +2390,16 @@
         <v>80</v>
       </c>
       <c r="B26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D26" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E26" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>246</v>
@@ -2516,93 +2408,105 @@
         <v>80</v>
       </c>
       <c r="H26" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>62</v>
+        <v>169</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="K26" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="L26" t="s">
-        <v>164</v>
+        <v>135</v>
       </c>
       <c r="M26" t="s">
-        <v>250</v>
-      </c>
-      <c r="N26" t="s">
-        <v>250</v>
-      </c>
-      <c r="O26" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B27" t="s">
         <v>80</v>
       </c>
       <c r="C27" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D27" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E27" t="s">
-        <v>58</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>248</v>
+        <v>10</v>
+      </c>
+      <c r="F27" t="s">
+        <v>258</v>
       </c>
       <c r="G27" s="12" t="s">
         <v>80</v>
       </c>
       <c r="H27" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="I27" t="s">
-        <v>186</v>
+        <v>180</v>
+      </c>
+      <c r="J27" t="s">
+        <v>183</v>
       </c>
       <c r="L27" t="s">
-        <v>164</v>
+        <v>135</v>
+      </c>
+      <c r="M27" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>80</v>
       </c>
-      <c r="B28" t="s">
-        <v>79</v>
+      <c r="B28" s="1" t="s">
+        <v>103</v>
       </c>
       <c r="C28" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D28" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="E28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F28" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="4" t="s">
         <v>246</v>
       </c>
       <c r="G28" s="12" t="s">
         <v>80</v>
       </c>
       <c r="H28" t="s">
-        <v>100</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>64</v>
+        <v>112</v>
+      </c>
+      <c r="I28" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="L28" t="s">
         <v>164</v>
       </c>
+      <c r="M28" t="s">
+        <v>184</v>
+      </c>
+      <c r="N28" t="s">
+        <v>184</v>
+      </c>
+      <c r="O28" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
@@ -2644,13 +2548,13 @@
         <v>80</v>
       </c>
       <c r="C30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D30" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="E30" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>246</v>
@@ -2659,103 +2563,88 @@
         <v>80</v>
       </c>
       <c r="H30" t="s">
-        <v>216</v>
+        <v>121</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="K30" t="s">
-        <v>204</v>
+        <v>82</v>
       </c>
       <c r="L30" t="s">
         <v>164</v>
       </c>
-      <c r="M30" t="s">
-        <v>203</v>
-      </c>
-      <c r="N30" t="s">
-        <v>203</v>
-      </c>
-      <c r="O30" t="s">
-        <v>160</v>
-      </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>80</v>
       </c>
       <c r="B31" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="C31" t="s">
-        <v>104</v>
+        <v>79</v>
       </c>
       <c r="D31" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E31" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G31" s="12" t="s">
         <v>80</v>
       </c>
       <c r="H31" t="s">
-        <v>118</v>
-      </c>
-      <c r="I31" t="s">
-        <v>188</v>
-      </c>
-      <c r="J31" t="s">
-        <v>189</v>
+        <v>122</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="L31" t="s">
         <v>164</v>
       </c>
-      <c r="M31" t="s">
-        <v>190</v>
-      </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B32" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
       <c r="C32" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
       <c r="D32" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E32" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G32" s="12" t="s">
         <v>80</v>
       </c>
       <c r="H32" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="I32" t="s">
-        <v>182</v>
+        <v>211</v>
+      </c>
+      <c r="J32" t="s">
+        <v>212</v>
       </c>
       <c r="L32" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M32" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B33" t="s">
         <v>104</v>
@@ -2764,65 +2653,77 @@
         <v>104</v>
       </c>
       <c r="D33" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E33" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G33" s="12" t="s">
         <v>80</v>
       </c>
       <c r="H33" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="I33" t="s">
-        <v>191</v>
+        <v>181</v>
+      </c>
+      <c r="J33" t="s">
+        <v>187</v>
       </c>
       <c r="L33" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M33" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>80</v>
       </c>
       <c r="B34" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C34" t="s">
         <v>79</v>
       </c>
       <c r="D34" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E34" t="s">
-        <v>28</v>
-      </c>
-      <c r="F34" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F34" s="5" t="s">
         <v>246</v>
       </c>
       <c r="G34" s="12" t="s">
         <v>80</v>
       </c>
       <c r="H34" t="s">
-        <v>121</v>
+        <v>222</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>82</v>
+        <v>73</v>
+      </c>
+      <c r="J34" s="5" t="s">
+        <v>215</v>
       </c>
       <c r="L34" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M34" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B35" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C35" t="s">
         <v>79</v>
@@ -2831,60 +2732,69 @@
         <v>30</v>
       </c>
       <c r="E35" t="s">
-        <v>34</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>242</v>
+        <v>38</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>246</v>
       </c>
       <c r="G35" s="12" t="s">
         <v>80</v>
       </c>
       <c r="H35" t="s">
-        <v>34</v>
-      </c>
-      <c r="I35" t="s">
-        <v>194</v>
-      </c>
-      <c r="J35" s="5" t="s">
-        <v>195</v>
+        <v>218</v>
+      </c>
+      <c r="I35" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="J35" s="7" t="s">
+        <v>77</v>
       </c>
       <c r="L35" t="s">
-        <v>164</v>
+        <v>199</v>
       </c>
       <c r="M35" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>80</v>
+      </c>
+      <c r="B36" t="s">
+        <v>79</v>
+      </c>
+      <c r="C36" t="s">
+        <v>80</v>
+      </c>
       <c r="D36" t="s">
         <v>30</v>
       </c>
       <c r="E36" t="s">
-        <v>259</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>242</v>
+        <v>39</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>246</v>
       </c>
       <c r="G36" s="12" t="s">
         <v>80</v>
       </c>
       <c r="H36" t="s">
-        <v>260</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="J36" t="s">
-        <v>152</v>
-      </c>
-      <c r="K36" t="s">
-        <v>152</v>
+        <v>219</v>
+      </c>
+      <c r="I36" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="J36" s="7" t="s">
+        <v>68</v>
       </c>
       <c r="L36" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M36" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>80</v>
       </c>
@@ -2892,33 +2802,39 @@
         <v>80</v>
       </c>
       <c r="C37" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D37" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E37" t="s">
-        <v>29</v>
-      </c>
-      <c r="F37" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F37" s="5" t="s">
         <v>246</v>
       </c>
       <c r="G37" s="12" t="s">
         <v>80</v>
       </c>
       <c r="H37" t="s">
-        <v>122</v>
-      </c>
-      <c r="I37" s="1" t="s">
-        <v>81</v>
+        <v>220</v>
+      </c>
+      <c r="I37" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="J37" s="7" t="s">
+        <v>70</v>
       </c>
       <c r="L37" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M37" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B38" t="s">
         <v>79</v>
@@ -2930,39 +2846,36 @@
         <v>30</v>
       </c>
       <c r="E38" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="G38" s="12" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H38" t="s">
-        <v>217</v>
-      </c>
-      <c r="I38" s="1" t="s">
-        <v>83</v>
+        <v>34</v>
+      </c>
+      <c r="I38" t="s">
+        <v>194</v>
+      </c>
+      <c r="J38" s="5" t="s">
+        <v>195</v>
       </c>
       <c r="L38" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>80</v>
-      </c>
-      <c r="B39" t="s">
-        <v>79</v>
-      </c>
-      <c r="C39" t="s">
-        <v>79</v>
-      </c>
+      <c r="M38" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D39" t="s">
         <v>30</v>
       </c>
       <c r="E39" t="s">
-        <v>37</v>
+        <v>259</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>242</v>
@@ -2971,27 +2884,27 @@
         <v>80</v>
       </c>
       <c r="H39" t="s">
-        <v>123</v>
-      </c>
-      <c r="I39" t="s">
-        <v>74</v>
+        <v>260</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>261</v>
       </c>
       <c r="J39" t="s">
-        <v>75</v>
+        <v>152</v>
+      </c>
+      <c r="K39" t="s">
+        <v>152</v>
       </c>
       <c r="L39" t="s">
-        <v>135</v>
-      </c>
-      <c r="M39" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>80</v>
       </c>
       <c r="B40" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C40" t="s">
         <v>79</v>
@@ -3000,27 +2913,27 @@
         <v>30</v>
       </c>
       <c r="E40" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F40" s="6" t="s">
         <v>246</v>
       </c>
       <c r="G40" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H40" t="s">
-        <v>32</v>
+        <v>217</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L40" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B41" t="s">
         <v>79</v>
@@ -3032,25 +2945,31 @@
         <v>30</v>
       </c>
       <c r="E41" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="G41" s="12" t="s">
         <v>80</v>
       </c>
       <c r="H41" t="s">
-        <v>33</v>
+        <v>123</v>
       </c>
       <c r="I41" t="s">
-        <v>193</v>
+        <v>74</v>
+      </c>
+      <c r="J41" t="s">
+        <v>75</v>
       </c>
       <c r="L41" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M41" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>80</v>
       </c>
@@ -3064,7 +2983,7 @@
         <v>30</v>
       </c>
       <c r="E42" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F42" s="6" t="s">
         <v>246</v>
@@ -3073,188 +2992,176 @@
         <v>80</v>
       </c>
       <c r="H42" t="s">
-        <v>221</v>
+        <v>32</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="J42" s="1" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="L42" t="s">
-        <v>197</v>
-      </c>
-      <c r="M42" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>79</v>
       </c>
       <c r="B43" t="s">
-        <v>104</v>
+        <v>79</v>
       </c>
       <c r="C43" t="s">
-        <v>104</v>
+        <v>79</v>
       </c>
       <c r="D43" t="s">
         <v>30</v>
       </c>
       <c r="E43" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="G43" s="12" t="s">
         <v>80</v>
       </c>
       <c r="H43" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="I43" t="s">
-        <v>88</v>
-      </c>
-      <c r="J43" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="L43" t="s">
-        <v>164</v>
-      </c>
-      <c r="M43" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B44" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="C44" t="s">
-        <v>104</v>
+        <v>79</v>
       </c>
       <c r="D44" t="s">
         <v>30</v>
       </c>
-      <c r="E44" s="2" t="s">
-        <v>42</v>
+      <c r="E44" t="s">
+        <v>35</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G44" s="12" t="s">
         <v>80</v>
       </c>
       <c r="H44" t="s">
-        <v>124</v>
-      </c>
-      <c r="I44" t="s">
-        <v>209</v>
+        <v>221</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="L44" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+        <v>197</v>
+      </c>
+      <c r="M44" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>79</v>
+      </c>
+      <c r="B45" t="s">
+        <v>104</v>
+      </c>
+      <c r="C45" t="s">
+        <v>104</v>
+      </c>
       <c r="D45" t="s">
         <v>30</v>
       </c>
-      <c r="E45" s="2" t="s">
-        <v>244</v>
+      <c r="E45" t="s">
+        <v>41</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="G45" s="12" t="s">
         <v>80</v>
       </c>
       <c r="H45" t="s">
+        <v>41</v>
+      </c>
+      <c r="I45" t="s">
+        <v>88</v>
+      </c>
+      <c r="J45" t="s">
+        <v>205</v>
+      </c>
+      <c r="L45" t="s">
+        <v>164</v>
+      </c>
+      <c r="M45" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>79</v>
+      </c>
+      <c r="B46" t="s">
         <v>104</v>
       </c>
-      <c r="I45" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>80</v>
-      </c>
-      <c r="B46" t="s">
-        <v>80</v>
-      </c>
       <c r="C46" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="D46" t="s">
-        <v>43</v>
-      </c>
-      <c r="E46" t="s">
-        <v>44</v>
-      </c>
-      <c r="F46" t="s">
-        <v>258</v>
+        <v>30</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>247</v>
       </c>
       <c r="G46" s="12" t="s">
         <v>80</v>
       </c>
       <c r="H46" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I46" t="s">
-        <v>85</v>
-      </c>
-      <c r="J46" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="L46" t="s">
         <v>164</v>
       </c>
-      <c r="M46" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>80</v>
-      </c>
-      <c r="B47" t="s">
-        <v>80</v>
-      </c>
-      <c r="C47" t="s">
-        <v>80</v>
-      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D47" t="s">
-        <v>43</v>
-      </c>
-      <c r="E47" t="s">
-        <v>45</v>
-      </c>
-      <c r="F47" t="s">
-        <v>258</v>
+        <v>30</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>242</v>
       </c>
       <c r="G47" s="12" t="s">
         <v>80</v>
       </c>
       <c r="H47" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="I47" t="s">
-        <v>86</v>
-      </c>
-      <c r="J47" t="s">
-        <v>207</v>
-      </c>
-      <c r="L47" t="s">
-        <v>164</v>
-      </c>
-      <c r="M47" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>80</v>
       </c>
@@ -3265,213 +3172,285 @@
         <v>80</v>
       </c>
       <c r="D48" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="E48" t="s">
-        <v>46</v>
-      </c>
-      <c r="F48" t="s">
-        <v>258</v>
+        <v>13</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>246</v>
       </c>
       <c r="G48" s="12" t="s">
         <v>80</v>
       </c>
       <c r="H48" t="s">
-        <v>127</v>
-      </c>
-      <c r="I48" t="s">
-        <v>87</v>
+        <v>113</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K48" t="s">
+        <v>185</v>
       </c>
       <c r="L48" t="s">
         <v>164</v>
       </c>
+      <c r="M48" t="s">
+        <v>250</v>
+      </c>
+      <c r="N48" t="s">
+        <v>250</v>
+      </c>
+      <c r="O48" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>79</v>
       </c>
       <c r="B49" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="C49" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="D49" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="E49" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="G49" s="12" t="s">
         <v>80</v>
       </c>
       <c r="H49" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="I49" t="s">
-        <v>214</v>
+        <v>186</v>
       </c>
       <c r="L49" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>80</v>
+      </c>
+      <c r="B50" t="s">
+        <v>79</v>
+      </c>
+      <c r="C50" t="s">
+        <v>79</v>
+      </c>
       <c r="D50" t="s">
-        <v>227</v>
+        <v>14</v>
       </c>
       <c r="E50" t="s">
-        <v>223</v>
-      </c>
-      <c r="F50" t="s">
-        <v>267</v>
+        <v>15</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>246</v>
       </c>
       <c r="G50" s="12" t="s">
         <v>80</v>
       </c>
       <c r="H50" t="s">
-        <v>229</v>
-      </c>
-      <c r="I50" t="s">
-        <v>234</v>
-      </c>
-      <c r="J50" t="s">
-        <v>236</v>
-      </c>
-      <c r="K50" t="s">
-        <v>240</v>
+        <v>100</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="L50" t="s">
         <v>164</v>
       </c>
-      <c r="M50" t="s">
-        <v>238</v>
-      </c>
-      <c r="N50" t="s">
-        <v>238</v>
-      </c>
-      <c r="O50" t="s">
-        <v>160</v>
-      </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>80</v>
+      </c>
+      <c r="B51" t="s">
+        <v>80</v>
+      </c>
+      <c r="C51" t="s">
+        <v>80</v>
+      </c>
       <c r="D51" t="s">
-        <v>227</v>
+        <v>14</v>
       </c>
       <c r="E51" t="s">
-        <v>224</v>
-      </c>
-      <c r="F51" t="s">
-        <v>267</v>
+        <v>16</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>246</v>
       </c>
       <c r="G51" s="12" t="s">
         <v>80</v>
       </c>
       <c r="H51" t="s">
-        <v>232</v>
-      </c>
-      <c r="I51" t="s">
-        <v>239</v>
+        <v>216</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K51" t="s">
+        <v>204</v>
       </c>
       <c r="L51" t="s">
         <v>164</v>
       </c>
+      <c r="M51" t="s">
+        <v>203</v>
+      </c>
+      <c r="N51" t="s">
+        <v>203</v>
+      </c>
+      <c r="O51" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>80</v>
+      </c>
+      <c r="B52" t="s">
+        <v>79</v>
+      </c>
+      <c r="C52" t="s">
+        <v>79</v>
+      </c>
       <c r="D52" t="s">
-        <v>227</v>
+        <v>20</v>
       </c>
       <c r="E52" t="s">
-        <v>225</v>
-      </c>
-      <c r="F52" t="s">
-        <v>267</v>
+        <v>21</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>246</v>
       </c>
       <c r="G52" s="12" t="s">
         <v>80</v>
       </c>
       <c r="H52" t="s">
-        <v>233</v>
-      </c>
-      <c r="I52" t="s">
-        <v>237</v>
+        <v>117</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="J52" s="5" t="s">
+        <v>252</v>
       </c>
       <c r="L52" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>80</v>
+      </c>
+      <c r="B53" t="s">
+        <v>104</v>
+      </c>
+      <c r="C53" t="s">
+        <v>104</v>
+      </c>
       <c r="D53" t="s">
-        <v>227</v>
+        <v>22</v>
       </c>
       <c r="E53" t="s">
-        <v>226</v>
-      </c>
-      <c r="F53" t="s">
-        <v>267</v>
+        <v>23</v>
+      </c>
+      <c r="F53" s="6" t="s">
+        <v>248</v>
       </c>
       <c r="G53" s="12" t="s">
         <v>80</v>
       </c>
       <c r="H53" t="s">
-        <v>230</v>
+        <v>118</v>
       </c>
       <c r="I53" t="s">
-        <v>235</v>
+        <v>188</v>
+      </c>
+      <c r="J53" t="s">
+        <v>189</v>
       </c>
       <c r="L53" t="s">
         <v>164</v>
       </c>
+      <c r="M53" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>80</v>
+      </c>
+      <c r="B54" t="s">
+        <v>79</v>
+      </c>
+      <c r="C54" t="s">
+        <v>79</v>
+      </c>
       <c r="D54" t="s">
-        <v>227</v>
+        <v>22</v>
       </c>
       <c r="E54" t="s">
-        <v>243</v>
+        <v>24</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>267</v>
+        <v>248</v>
       </c>
       <c r="G54" s="12" t="s">
         <v>80</v>
       </c>
       <c r="H54" t="s">
+        <v>119</v>
+      </c>
+      <c r="I54" t="s">
+        <v>182</v>
+      </c>
+      <c r="L54" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>80</v>
+      </c>
+      <c r="B55" t="s">
         <v>104</v>
       </c>
-      <c r="I54" t="s">
-        <v>269</v>
-      </c>
-      <c r="J54" t="s">
-        <v>270</v>
-      </c>
-      <c r="L54" t="s">
-        <v>271</v>
-      </c>
-      <c r="M54" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C55" t="s">
+        <v>104</v>
+      </c>
       <c r="D55" t="s">
-        <v>227</v>
+        <v>22</v>
       </c>
       <c r="E55" t="s">
-        <v>228</v>
-      </c>
-      <c r="F55" t="s">
-        <v>267</v>
+        <v>25</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>248</v>
       </c>
       <c r="G55" s="12" t="s">
         <v>80</v>
       </c>
       <c r="H55" t="s">
-        <v>231</v>
+        <v>120</v>
       </c>
       <c r="I55" t="s">
-        <v>241</v>
+        <v>191</v>
       </c>
       <c r="L55" t="s">
         <v>164</v>
@@ -3535,7 +3514,7 @@
       </c>
       <c r="B3">
         <f>COUNTIF(Manifest!$F$2:$F$55,A3)</f>
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C3">
         <v>18</v>
@@ -3550,7 +3529,7 @@
       </c>
       <c r="B4">
         <f>COUNTIF(Manifest!$F$2:$F$55,A4)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -3610,7 +3589,7 @@
       </c>
       <c r="B8" s="10">
         <f>COUNTIF(Manifest!$F$2:$F$55,A8)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C8" s="10">
         <v>3</v>
@@ -3625,7 +3604,7 @@
       </c>
       <c r="B9">
         <f>SUM(B2:B8)</f>
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9">
         <f t="shared" ref="C9:D9" si="0">SUM(C2:C8)</f>
@@ -3639,11 +3618,11 @@
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C10" s="9">
         <f>C9/B9</f>
-        <v>0.97916666666666663</v>
+        <v>1</v>
       </c>
       <c r="D10" s="9">
         <f>D9/B9</f>
-        <v>0.66666666666666663</v>
+        <v>0.68085106382978722</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>